<commit_message>
Update Overview information and debug spec
</commit_message>
<xml_diff>
--- a/001_General_Spec/VG_Oveview_Information.xlsx
+++ b/001_General_Spec/VG_Oveview_Information.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="129">
   <si>
     <t>Ký hiệu hoặc viết tắt</t>
   </si>
@@ -406,6 +406,18 @@
   </si>
   <si>
     <t>Nguyễn Phong</t>
+  </si>
+  <si>
+    <t>VGA</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>RESET</t>
   </si>
 </sst>
 </file>
@@ -550,7 +562,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1636,10 +1658,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -1655,7 +1677,7 @@
     <col min="9" max="9" width="11" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="11"/>
     <col min="11" max="11" width="11.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.2109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.0703125" style="11" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
@@ -2037,75 +2059,382 @@
       </c>
       <c r="L12" s="13"/>
     </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
+        <v>17</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="3">
+        <v>21</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="3">
+        <v>23</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
+        <v>25</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
+        <v>27</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="H3:XFD3 A3:G6 A8:G8">
-    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
+  <conditionalFormatting sqref="H3:XFD3 A3:G4 B8:G8 B5:G6 A5:A29">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:XFD6 H8:J8 L8:XFD8">
-    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:G7 A9">
-    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
+  <conditionalFormatting sqref="B7:G7">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:J7 M7:XFD7">
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:G9">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:J9 L9:XFD9">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>